<commit_message>
받으시면 FSM.ipynb에 answer_data 다시넣기
</commit_message>
<xml_diff>
--- a/train_tools/qna/Answer_data.xlsx
+++ b/train_tools/qna/Answer_data.xlsx
@@ -77,17 +77,6 @@
 {B_FOOD} 주문, {B_FOOD} 줘</t>
   </si>
   <si>
-    <t>추가 옵션을 선택해주세요
-없으시다면 0을 입력해주세요
-1 = 샷추가
-2 = 시럽추가
-3 = 사이즈업
-4 = 샷 + 시럽추가
-5 = 샷 + 사이즈업
-6 = 시럽 + 사이즈업
-7 = 샷 + 시럽 + 사이즈업</t>
-  </si>
-  <si>
     <t>추천메뉴</t>
   </si>
   <si>
@@ -353,12 +342,341 @@
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t>추가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>옵션을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">선택해주세요
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1 = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">옵션없음
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2 = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">샷추가
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">3 = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">시럽추가
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">4 = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">사이즈업
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">5 = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>샷</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">시럽추가
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">6 = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>샷</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">사이즈업
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">7 = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>시럽</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">사이즈업
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">8 = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>샷</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>시럽</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>사이즈업</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -417,6 +735,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -630,7 +956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -690,6 +1016,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -910,7 +1239,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -956,7 +1285,7 @@
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="136.5" thickBot="1">
@@ -969,48 +1298,48 @@
       <c r="C3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>20</v>
+      <c r="D3" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" ht="48" thickBot="1">
       <c r="A4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="10" t="s">
         <v>23</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>24</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" ht="48" thickBot="1">
       <c r="A5" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>28</v>
-      </c>
       <c r="F5" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="64.5" thickBot="1">
@@ -1019,70 +1348,70 @@
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>29</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>30</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="294" thickBot="1">
       <c r="A7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:6" ht="138.75" thickBot="1">
       <c r="A8" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" ht="33" thickBot="1">
       <c r="A9" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" ht="79.5" thickBot="1">
       <c r="A10" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
@@ -1098,7 +1427,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
login 반영 후 cafebot 엔진 8차 수정
</commit_message>
<xml_diff>
--- a/train_tools/qna/Answer_data.xlsx
+++ b/train_tools/qna/Answer_data.xlsx
@@ -160,9 +160,6 @@
     <t>테이크 아웃 설명입니다</t>
   </si>
   <si>
-    <t>해당 {B_FOOD}의 주문번호를 입력해주세요</t>
-  </si>
-  <si>
     <t>PrintedMenus.png</t>
   </si>
   <si>
@@ -516,6 +513,83 @@
 7 = 시럽 + 사이즈업
 8 = 샷 + 시럽 + 사이즈업
 ===========================</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>해당</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>상품의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>주문번호를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>입력해주세요</t>
+    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -856,9 +930,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -866,6 +937,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1085,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1132,7 +1206,7 @@
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="241.5" thickBot="1">
@@ -1145,11 +1219,11 @@
       <c r="C3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="21" t="s">
-        <v>45</v>
+      <c r="D3" s="20" t="s">
+        <v>44</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3" s="13"/>
     </row>
@@ -1177,16 +1251,16 @@
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="64.5" thickBot="1">
@@ -1273,13 +1347,13 @@
       <c r="C11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="19" t="s">
+      <c r="D11" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="20"/>
+      <c r="F11" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>